<commit_message>
Change accuracy measure to informedness (balanced_accuracy)
</commit_message>
<xml_diff>
--- a/model_results.xlsx
+++ b/model_results.xlsx
@@ -43,7 +43,7 @@
     <t>XGBoost</t>
   </si>
   <si>
-    <t>{'clf__criterion': 'gini', 'clf__max_depth': 7, 'clf__min_samples_leaf': 3, 'clf__min_samples_split': 0.05}</t>
+    <t>{'clf__criterion': 'gini', 'clf__max_depth': 9, 'clf__min_samples_leaf': 3, 'clf__min_samples_split': 0.05}</t>
   </si>
   <si>
     <t>{'logreg__C': 100, 'logreg__penalty': 'l1'}</t>
@@ -52,7 +52,7 @@
     <t>{'svm__C': 10, 'svm__degree': 1, 'svm__gamma': 'auto', 'svm__kernel': 'rbf'}</t>
   </si>
   <si>
-    <t>{'rf__criterion': 'gini', 'rf__max_depth': 9, 'rf__min_samples_leaf': 3, 'rf__min_samples_split': 0.05}</t>
+    <t>{'rf__criterion': 'entropy', 'rf__max_depth': 9, 'rf__min_samples_leaf': 1, 'rf__min_samples_split': 0.05}</t>
   </si>
   <si>
     <t>{'ada__learning_rate': 0.39}</t>
@@ -441,7 +441,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.7113207547169811</v>
+        <v>0.6980567603353105</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -455,7 +455,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.8056603773584906</v>
+        <v>0.80642373817349</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -469,7 +469,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0.9018867924528302</v>
+        <v>0.9060831631487044</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -483,7 +483,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0.7849056603773585</v>
+        <v>0.7733390130674143</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -497,7 +497,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0.7075471698113207</v>
+        <v>0.7024704789650172</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -511,7 +511,7 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0.8641509433962264</v>
+        <v>0.8580617694972213</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>

</xml_diff>